<commit_message>
Finished with creation of xls
</commit_message>
<xml_diff>
--- a/Təkliflərin reyestri1.xlsx
+++ b/Təkliflərin reyestri1.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="41">
   <si>
     <t>Büdcə təşkilatları tərəfindən vergi və gömrük sahəsində verilmiş müraciətlərə baxılmanın nəticələri haqqında hesabat</t>
   </si>
@@ -131,6 +131,36 @@
   </si>
   <si>
     <t>document</t>
+  </si>
+  <si>
+    <t>activity1</t>
+  </si>
+  <si>
+    <t>Discount</t>
+  </si>
+  <si>
+    <t>Unknown Aim</t>
+  </si>
+  <si>
+    <t>10 hours</t>
+  </si>
+  <si>
+    <t>No type</t>
+  </si>
+  <si>
+    <t>No additional income</t>
+  </si>
+  <si>
+    <t>No impact</t>
+  </si>
+  <si>
+    <t>active</t>
+  </si>
+  <si>
+    <t>saa123321</t>
+  </si>
+  <si>
+    <t>1000 AZN</t>
   </si>
 </sst>
 </file>
@@ -138,7 +168,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -157,6 +187,11 @@
       <sz val="12.0"/>
       <color indexed="8"/>
       <b val="true"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <sz val="12.0"/>
+      <color indexed="8"/>
     </font>
   </fonts>
   <fills count="4">
@@ -207,10 +242,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFill="true" applyFont="true" applyBorder="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -219,7 +257,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -363,71 +401,139 @@
       </c>
     </row>
     <row r="4" ht="64.0" customHeight="true">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="3" t="n">
+        <v>738118.0</v>
+      </c>
+      <c r="G4" s="3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="S4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="T4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>26</v>
+      <c r="P4" s="3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" ht="64.0" customHeight="true">
+      <c r="A5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <v>738118.0</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>1000.0</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" s="3" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="3" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>